<commit_message>
Chris Transportation updates for AVIC, AVLRaPTC, AVMC, BBSoEVP, BESP, BMRESP, BNVP, SoCDTtiNTY, TTS
</commit_message>
<xml_diff>
--- a/InputData/trans/AVIC/Annual Vehicle Insurance Cost.xlsx
+++ b/InputData/trans/AVIC/Annual Vehicle Insurance Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\AVIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\Current CA EPS update\Revised variables\Transpo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C68CA1-D4E5-4267-A93A-22A2147EC345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE19E89D-4F29-43B2-B86B-D6BA5AE15838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="1470" windowWidth="22500" windowHeight="21135" xr2:uid="{D78DFE5E-0A7F-4A12-AD34-4FEABB0CFCE7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D78DFE5E-0A7F-4A12-AD34-4FEABB0CFCE7}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -656,19 +656,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC790369-4F84-43C0-97E9-6D0C01E4139F}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -676,177 +676,177 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>2021</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B24" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>2021</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.89800000000000002</v>
       </c>
@@ -854,7 +854,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>0.88700000000000001</v>
       </c>
@@ -862,7 +862,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="10">
         <f>A47/(1+A50)</f>
         <v>0.83052434456928836</v>
@@ -871,7 +871,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="9">
         <v>6.8000000000000005E-2</v>
       </c>
@@ -898,25 +898,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -927,19 +927,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -950,7 +950,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -968,7 +968,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -986,7 +986,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1040,19 +1040,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1098,24 +1098,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1126,19 +1126,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -1161,15 +1161,17 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="3" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>69</v>
       </c>
@@ -1180,7 +1182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1193,7 +1195,7 @@
         <v>3944.9906367041199</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1206,7 +1208,7 @@
         <v>8082.6629213483147</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1228,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1239,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1247,8 +1249,9 @@
         <f>Data!B37*About!A48</f>
         <v>598.80805243445695</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" s="11">
+        <f>$C$3</f>
+        <v>8082.6629213483147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>